<commit_message>
fixed NA problem in bcilist
</commit_message>
<xml_diff>
--- a/splists_out/Plantnet species/BCI_SPECIES_LIST_POSSIBLY_WOODY_2026-02-25.xlsx
+++ b/splists_out/Plantnet species/BCI_SPECIES_LIST_POSSIBLY_WOODY_2026-02-25.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5085,39 +5085,24 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Musa paradisiaca</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>Musa × paradisiaca</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>Musa paradisiaca</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>Musaceae</t>
+          <t>Monstera involuta</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>herbaceous tree</t>
+          <t>shrub</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Musa sapientum</t>
+          <t>Musa paradisiaca</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Musa × sapientum</t>
+          <t>Musa × paradisiaca</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -5139,76 +5124,76 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Nectandra globosa</t>
+          <t>Musa sapientum</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Nectandra globosa</t>
+          <t>Musa × sapientum</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Nectandra globosa</t>
+          <t>Musa paradisiaca</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Lauraceae</t>
+          <t>Musaceae</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>tree</t>
+          <t>herbaceous tree</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Neea pittieri</t>
+          <t>Nectandra globosa</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Neea pittieri</t>
+          <t>Nectandra globosa</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Neea pittieri</t>
+          <t>Nectandra globosa</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Nyctaginaceae</t>
+          <t>Lauraceae</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>shrub or tree</t>
+          <t>tree</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Ormosia coccinea var. subsimplex</t>
+          <t>Neea pittieri</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Ormosia coccinea var. subsimplex</t>
+          <t>Neea pittieri</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Ormosia subsimplex</t>
+          <t>Neea pittieri</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Nyctaginaceae</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -5220,98 +5205,98 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Palicourea cuspidata</t>
+          <t>Ormosia coccinea var. subsimplex</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Palicourea cuspidata</t>
+          <t>Ormosia coccinea var. subsimplex</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Palicourea cuspidata</t>
+          <t>Ormosia subsimplex</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Rubiaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>shrub</t>
+          <t>shrub or tree</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Pavonia rosea</t>
+          <t>Palicourea cuspidata</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Pavonia rosea</t>
+          <t>Palicourea cuspidata</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Pavonia leptocalyx</t>
+          <t>Palicourea cuspidata</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Malvaceae</t>
+          <t>Rubiaceae</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>subshrub or shrub</t>
+          <t>shrub</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Piper albopunctulatissimum</t>
+          <t>Pavonia rosea</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Piper albopunctulatissimum</t>
+          <t>Pavonia rosea</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Piper albopunctulatissimum</t>
+          <t>Pavonia leptocalyx</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>Piperaceae</t>
+          <t>Malvaceae</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>shrub or tree</t>
+          <t>subshrub or shrub</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Piper amphioxys</t>
+          <t>Piper albopunctulatissimum</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Piper amphioxys</t>
+          <t>Piper albopunctulatissimum</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Piper amphioxys</t>
+          <t>Piper albopunctulatissimum</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -5321,24 +5306,24 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>shrub</t>
+          <t>shrub or tree</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Piper biauritum</t>
+          <t>Piper amphioxys</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Piper biauritum</t>
+          <t>Piper amphioxys</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Piper biauritum</t>
+          <t>Piper amphioxys</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -5355,17 +5340,17 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Piper cabagranum</t>
+          <t>Piper biauritum</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Piper cabagranum</t>
+          <t>Piper biauritum</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Piper cabagranum</t>
+          <t>Piper biauritum</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -5382,17 +5367,17 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Piper casimiranum</t>
+          <t>Piper cabagranum</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Piper casimirianum</t>
+          <t>Piper cabagranum</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Piper casimirianum</t>
+          <t>Piper cabagranum</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -5402,24 +5387,24 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>subshrub or shrub</t>
+          <t>shrub</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Piper leptocladum</t>
+          <t>Piper casimiranum</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Piper leptocladum</t>
+          <t>Piper casimirianum</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Piper leptocladum</t>
+          <t>Piper casimirianum</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -5429,24 +5414,24 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>shrub</t>
+          <t>subshrub or shrub</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Piper playablancanum</t>
+          <t>Piper leptocladum</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Piper playa-blancanum</t>
+          <t>Piper leptocladum</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Piper playa-blancanum</t>
+          <t>Piper leptocladum</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -5456,24 +5441,24 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>subshrub or shrub</t>
+          <t>shrub</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Piper pseudovariabile</t>
+          <t>Piper playablancanum</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Piper pseudovariabile</t>
+          <t>Piper playa-blancanum</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Piper pseudovariabile</t>
+          <t>Piper playa-blancanum</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -5483,24 +5468,24 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>shrub</t>
+          <t>subshrub or shrub</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Piper schiedeanum</t>
+          <t>Piper pseudovariabile</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Piper schiedeanum</t>
+          <t>Piper pseudovariabile</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Piper schiedeanum</t>
+          <t>Piper pseudovariabile</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -5510,24 +5495,24 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>shrub or tree</t>
+          <t>shrub</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Piper seducentifolium</t>
+          <t>Piper schiedeanum</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Piper seducentifolium</t>
+          <t>Piper schiedeanum</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Piper seducentifolium</t>
+          <t>Piper schiedeanum</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -5537,78 +5522,78 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>subshrub or shrub</t>
+          <t>shrub or tree</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Pogonopus speciosus</t>
+          <t>Piper seducentifolium</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Pogonopus speciosus</t>
+          <t>Piper seducentifolium</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Pogonopus speciosus</t>
+          <t>Piper seducentifolium</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Rubiaceae</t>
+          <t>Piperaceae</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>shrub or tree</t>
+          <t>subshrub or shrub</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Pouteria glomerata</t>
+          <t>Pogonopus speciosus</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Pouteria glomerata</t>
+          <t>Pogonopus speciosus</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Pouteria glomerata</t>
+          <t>Pogonopus speciosus</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Sapotaceae</t>
+          <t>Rubiaceae</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>tree</t>
+          <t>shrub or tree</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Pouteria glomerata subsp. stylosa</t>
+          <t>Pouteria glomerata</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Pouteria glomerata subsp. stylosa</t>
+          <t>Pouteria glomerata</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Pouteria glomerata subsp. stylosa</t>
+          <t>Pouteria glomerata</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -5625,49 +5610,49 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Psychotria patens</t>
+          <t>Pouteria glomerata subsp. stylosa</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Psychotria patens</t>
+          <t>Pouteria glomerata subsp. stylosa</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Palicourea patens</t>
+          <t>Pouteria glomerata subsp. stylosa</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Rubiaceae</t>
+          <t>Sapotaceae</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>shrub</t>
+          <t>tree</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Rosa spinosissima</t>
+          <t>Psychotria patens</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Rosa spinosissima</t>
+          <t>Psychotria patens</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Rosa spinosissima</t>
+          <t>Palicourea patens</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Rubiaceae</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -5679,44 +5664,44 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Senna bacillaris var. bacillaris</t>
+          <t>Rosa spinosissima</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Senna bacillaris var. bacillaris</t>
+          <t>Rosa spinosissima</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Senna bacillaris var. bacillaris</t>
+          <t>Rosa spinosissima</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>shrub or tree</t>
+          <t>shrub</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Senna dariensis var. dariensis</t>
+          <t>Senna bacillaris var. bacillaris</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Senna dariensis var. dariensis</t>
+          <t>Senna bacillaris var. bacillaris</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Senna dariensis var. dariensis</t>
+          <t>Senna bacillaris var. bacillaris</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -5733,76 +5718,76 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Stictocardia tiliifolia subsp. tiliifolia</t>
+          <t>Senna dariensis var. dariensis</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Stictocardia tiliifolia subsp. tiliifolia</t>
+          <t>Senna dariensis var. dariensis</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Stictocardia tiliifolia subsp. tiliifolia</t>
+          <t>Senna dariensis var. dariensis</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Convolvulaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>liana</t>
+          <t>shrub or tree</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Syzygium melanostictum</t>
+          <t>Stictocardia tiliifolia subsp. tiliifolia</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Syzygium melanostictum</t>
+          <t>Stictocardia tiliifolia subsp. tiliifolia</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Syzygium melanostictum</t>
+          <t>Stictocardia tiliifolia subsp. tiliifolia</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Myrtaceae</t>
+          <t>Convolvulaceae</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>tree</t>
+          <t>liana</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Talisia princeps</t>
+          <t>Syzygium melanostictum</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Talisia princeps</t>
+          <t>Syzygium melanostictum</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Talisia princeps</t>
+          <t>Syzygium melanostictum</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Sapindaceae</t>
+          <t>Myrtaceae</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
@@ -5814,34 +5799,34 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Tetracera costata</t>
+          <t>Talisia princeps</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Tetracera costata</t>
+          <t>Talisia princeps</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Tetracera costata</t>
+          <t>Talisia princeps</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Dilleniaceae</t>
+          <t>Sapindaceae</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>liana</t>
+          <t>tree</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Tetracera costata subsp. costata</t>
+          <t>Tetracera costata</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -5861,24 +5846,24 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>tree</t>
+          <t>liana</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Tetracera volubilis subsp. volubilis</t>
+          <t>Tetracera costata subsp. costata</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Tetracera volubilis subsp. volubilis</t>
+          <t>Tetracera costata</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Tetracera volubilis subsp. volubilis</t>
+          <t>Tetracera costata</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -5888,110 +5873,110 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>liana</t>
+          <t>tree</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Trichilia cipo</t>
+          <t>Tetracera volubilis subsp. volubilis</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Trichilia cipo</t>
+          <t>Tetracera volubilis subsp. volubilis</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Trichilia cipo</t>
+          <t>Tetracera volubilis subsp. volubilis</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Meliaceae</t>
+          <t>Dilleniaceae</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>tree</t>
+          <t>liana</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Urena lobata</t>
+          <t>Trichilia cipo</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Urena lobata</t>
+          <t>Trichilia cipo</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Urena lobata</t>
+          <t>Trichilia cipo</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Malvaceae</t>
+          <t>Meliaceae</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>subshrub or shrub</t>
+          <t>tree</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Vachellia cornigera</t>
+          <t>Urena lobata</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Vachellia cornigera</t>
+          <t>Urena lobata</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Vachellia cornigera</t>
+          <t>Urena lobata</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Malvaceae</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>shrub or tree</t>
+          <t>subshrub or shrub</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Vismia guianensis</t>
+          <t>Vachellia cornigera</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Vismia guianensis</t>
+          <t>Vachellia cornigera</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Vismia guianensis</t>
+          <t>Vachellia cornigera</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Hypericaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
@@ -6003,17 +5988,17 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Vismia latifolia</t>
+          <t>Vismia guianensis</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Vismia latifolia</t>
+          <t>Vismia guianensis</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Vismia latifolia</t>
+          <t>Vismia guianensis</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -6023,32 +6008,59 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>tree</t>
+          <t>shrub or tree</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
+          <t>Vismia latifolia</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Vismia latifolia</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Vismia latifolia</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Hypericaceae</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>tree</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
           <t>Zygia latifolia var. latifolia</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr">
+      <c r="B212" t="inlineStr">
         <is>
           <t>Zygia latifolia var. latifolia</t>
         </is>
       </c>
-      <c r="C211" t="inlineStr">
+      <c r="C212" t="inlineStr">
         <is>
           <t>Zygia latifolia var. latifolia</t>
         </is>
       </c>
-      <c r="D211" t="inlineStr">
+      <c r="D212" t="inlineStr">
         <is>
           <t>Fabaceae</t>
         </is>
       </c>
-      <c r="E211" t="inlineStr">
+      <c r="E212" t="inlineStr">
         <is>
           <t>shrub or tree</t>
         </is>

</xml_diff>